<commit_message>
Child level analysis - truncated
</commit_message>
<xml_diff>
--- a/Code/Graphs.xlsx
+++ b/Code/Graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="28220" windowHeight="16420" activeTab="3"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="26500" windowHeight="16420" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ASER Results" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,13 @@
     <sheet name="MELQO" sheetId="3" r:id="rId3"/>
     <sheet name="MELQO Child" sheetId="8" r:id="rId4"/>
     <sheet name="truncated sample" sheetId="4" r:id="rId5"/>
-    <sheet name="Balance Test" sheetId="2" r:id="rId6"/>
-    <sheet name="viz" sheetId="5" r:id="rId7"/>
-    <sheet name="top 20%" sheetId="6" r:id="rId8"/>
+    <sheet name="Truncated Child" sheetId="9" r:id="rId6"/>
+    <sheet name="Balance Test" sheetId="2" r:id="rId7"/>
+    <sheet name="viz" sheetId="5" r:id="rId8"/>
+    <sheet name="top 20%" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'top 20%'!$A$3:$A$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'top 20%'!$A$3:$A$3</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="59">
   <si>
     <t>English</t>
   </si>
@@ -1618,6 +1619,1063 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Truncated Child'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grade 1 - 3 Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Truncated Child'!$B$5:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>English</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Maths</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Urdu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Truncated Child'!$C$5:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.2135</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.3800000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D480-454C-AEDB-1FB834A6504C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Truncated Child'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grade 1 - 3 Endline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Truncated Child'!$B$5:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>English</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Maths</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Urdu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Truncated Child'!$D$5:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.2999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0000000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D480-454C-AEDB-1FB834A6504C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1146675567"/>
+        <c:axId val="1146347839"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1146675567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1146347839"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1146347839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1146675567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Truncated Child'!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grade 4 - 5 Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Truncated Child'!$B$12:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>English</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Maths</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Urdu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Truncated Child'!$C$12:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23880000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1429</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-186B-9B4D-991B-4417B2F1F426}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Truncated Child'!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grade 4 - 5 Endline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Truncated Child'!$B$12:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>English</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Maths</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Urdu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Truncated Child'!$D$12:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.10630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.58E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21240000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-186B-9B4D-991B-4417B2F1F426}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1143337567"/>
+        <c:axId val="1143032271"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1143337567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1143032271"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1143032271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1143337567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Truncated Child'!$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Truncated Child'!$B$18:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pre-Literacy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pre-Numeracy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Motor Skills</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Truncated Child'!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.8300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3200000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8799999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A986-E34A-8F6C-AF211CF8AEA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Truncated Child'!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Endline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Truncated Child'!$B$18:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pre-Literacy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pre-Numeracy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Motor Skills</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Truncated Child'!$D$18:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.5300000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1399999999999995E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A986-E34A-8F6C-AF211CF8AEA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="707664735"/>
+        <c:axId val="707359711"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="707664735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="707359711"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="707359711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="707664735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -1775,145 +2833,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2837-A848-9F49-A9DF95EFDAA9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ASER Results'!$X$1:$X$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Taleemabad</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4 - 5 Baseline</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ASER Results'!$U$3:$U$5</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>English</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Maths</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Urdu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ASER Results'!$X$3:$X$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.6E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-8.6999999999999994E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2837-A848-9F49-A9DF95EFDAA9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ASER Results'!$Y$1:$Y$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Taleemabad</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4 - 5 Endline</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ASER Results'!$U$3:$U$5</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>English</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Maths</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Urdu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ASER Results'!$Y$3:$Y$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>3.5999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.4999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.1999999999999999E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-2837-A848-9F49-A9DF95EFDAA9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1982,7 +2901,7 @@
         <c:axId val="812853552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-0.1"/>
+          <c:min val="-5.000000000000001E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2281,145 +3200,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ASER Results'!$Q$1:$Q$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Taleemabad</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 - 3 Baseline</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ASER Results'!$N$3:$N$5</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>English</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Maths</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Urdu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ASER Results'!$Q$3:$Q$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>-7.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.7999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.13600000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4ED4-384B-B505-C349640CB2E9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ASER Results'!$R$1:$R$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Taleemabad</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 - 3 Endline</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ASER Results'!$N$3:$N$5</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>English</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Maths</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Urdu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ASER Results'!$R$3:$R$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.22900000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.9000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.14599999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-4ED4-384B-B505-C349640CB2E9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2485,7 +3265,7 @@
         <c:axId val="540397360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-0.15000000000000002"/>
+          <c:min val="-5.000000000000001E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2537,6 +3317,7 @@
         <c:crossAx val="545925280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3724,7 +4505,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3838,12 +4622,14 @@
         <c:axId val="164720512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="6.0000000000000012E-2"/>
+          <c:min val="-1.0000000000000002E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -3891,7 +4677,7 @@
         <c:crossAx val="269527024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2.0000000000000004E-2"/>
+        <c:majorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5414,6 +6200,126 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7273,6 +8179,1515 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -11337,15 +13752,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>143933</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>558799</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>59266</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>338667</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>694267</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11379,10 +13794,10 @@
       <xdr:rowOff>8466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>169333</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11497,10 +13912,10 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>186266</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11718,6 +14133,119 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D25207A-E90A-5B48-A13D-CE07B350B851}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58CFB7A9-CC79-254A-9823-0DF7BB2A261E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E10BDD-1C78-2747-9A0C-4DCC77BBFB9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -12017,8 +14545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:Y5"/>
+    <sheetView topLeftCell="K1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12045,9 +14573,7 @@
         <v>24</v>
       </c>
       <c r="P1" s="24"/>
-      <c r="Q1" s="24" t="s">
-        <v>25</v>
-      </c>
+      <c r="Q1" s="24"/>
       <c r="R1" s="24"/>
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
@@ -12055,9 +14581,7 @@
         <v>24</v>
       </c>
       <c r="W1" s="24"/>
-      <c r="X1" s="24" t="s">
-        <v>25</v>
-      </c>
+      <c r="X1" s="24"/>
       <c r="Y1" s="24"/>
     </row>
     <row r="2" spans="2:25">
@@ -12093,12 +14617,8 @@
       <c r="P2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -12108,12 +14628,8 @@
       <c r="W2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="2:25">
       <c r="B3" s="1" t="s">
@@ -12153,12 +14669,8 @@
       <c r="P3" s="12">
         <v>0.17249999999999999</v>
       </c>
-      <c r="Q3" s="14">
-        <v>-7.0000000000000001E-3</v>
-      </c>
-      <c r="R3" s="14">
-        <v>0.22900000000000001</v>
-      </c>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
       <c r="S3" s="14"/>
       <c r="T3" s="14"/>
       <c r="U3" s="1" t="s">
@@ -12171,12 +14683,8 @@
         <f>2.55/100</f>
         <v>2.5499999999999998E-2</v>
       </c>
-      <c r="X3" s="14">
-        <v>1.6E-2</v>
-      </c>
-      <c r="Y3" s="14">
-        <v>3.5999999999999997E-2</v>
-      </c>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="2:25">
       <c r="B4" s="1" t="s">
@@ -12221,12 +14729,8 @@
         <f>-3.17/100</f>
         <v>-3.1699999999999999E-2</v>
       </c>
-      <c r="Q4" s="14">
-        <v>-1.7999999999999999E-2</v>
-      </c>
-      <c r="R4" s="14">
-        <v>-2.9000000000000001E-2</v>
-      </c>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
       <c r="U4" s="1" t="s">
@@ -12240,12 +14744,8 @@
         <f>4.77/100</f>
         <v>4.7699999999999992E-2</v>
       </c>
-      <c r="X4" s="14">
-        <v>1.9E-2</v>
-      </c>
-      <c r="Y4" s="14">
-        <v>1.4999999999999999E-2</v>
-      </c>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
     </row>
     <row r="5" spans="2:25">
       <c r="B5" s="1" t="s">
@@ -12290,12 +14790,8 @@
         <f>8.285/100</f>
         <v>8.2850000000000007E-2</v>
       </c>
-      <c r="Q5" s="14">
-        <v>-0.13600000000000001</v>
-      </c>
-      <c r="R5" s="14">
-        <v>0.14599999999999999</v>
-      </c>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
       <c r="U5" s="1" t="s">
@@ -12309,12 +14805,8 @@
         <f>13.48/100</f>
         <v>0.1348</v>
       </c>
-      <c r="X5" s="14">
-        <v>-8.6999999999999994E-2</v>
-      </c>
-      <c r="Y5" s="14">
-        <v>2.1999999999999999E-2</v>
-      </c>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
     </row>
     <row r="6" spans="2:25">
       <c r="B6" s="1"/>
@@ -12540,7 +15032,7 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F6"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12641,7 +15133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -12740,8 +15232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12915,6 +15407,168 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.2135</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12">
+        <v>-2.3800000000000002E-2</v>
+      </c>
+      <c r="D6" s="13">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.1101</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="12">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.10630000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.23880000000000001</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2.58E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.1429</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.21240000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="12">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="D18" s="12">
+        <v>7.5300000000000006E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="12">
+        <v>6.3200000000000006E-2</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="12">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="D20" s="12">
+        <v>9.1399999999999995E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H23"/>
   <sheetViews>
@@ -13309,7 +15963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J13"/>
   <sheetViews>
@@ -13629,7 +16283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O21"/>
   <sheetViews>

</xml_diff>

<commit_message>
school level analysis added in 2_analysis
</commit_message>
<xml_diff>
--- a/Code/Graphs.xlsx
+++ b/Code/Graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="26500" windowHeight="16420" activeTab="5"/>
+    <workbookView xWindow="1560" yWindow="540" windowWidth="17480" windowHeight="16420" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ASER Results" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="63">
   <si>
     <t>English</t>
   </si>
@@ -213,6 +213,18 @@
   <si>
     <t>pre literacy</t>
   </si>
+  <si>
+    <t>full sample</t>
+  </si>
+  <si>
+    <t>Full sample - school level</t>
+  </si>
+  <si>
+    <t>Full sample - child level</t>
+  </si>
+  <si>
+    <t>in the consistent schools</t>
+  </si>
 </sst>
 </file>
 
@@ -337,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -403,6 +415,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,12 +1245,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1481,6 +1490,7 @@
         <c:axId val="546978144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="8.0000000000000016E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1588,12 +1598,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -3009,12 +3014,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -3374,12 +3374,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -6091,12 +6086,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -13755,13 +13745,13 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>558799</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>59266</xdr:rowOff>
+      <xdr:rowOff>59265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>694267</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>16934</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>67732</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14030,10 +14020,10 @@
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14061,15 +14051,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14545,7 +14535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y8"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="75" workbookViewId="0">
       <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
@@ -15032,7 +15022,7 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15232,8 +15222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15410,7 +15400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -15570,10 +15560,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H23"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:G23"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16"/>
@@ -15582,10 +15572,26 @@
     <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="7" width="11.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="15.83203125" style="1"/>
+    <col min="8" max="8" width="15.83203125" style="1"/>
+    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="1" customWidth="1"/>
+    <col min="11" max="14" width="11.83203125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="15.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="20" customHeight="1">
+    <row r="1" spans="1:14">
+      <c r="D1" s="32"/>
+      <c r="I1" s="32"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="20" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2"/>
@@ -15598,8 +15604,18 @@
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="20" customHeight="1">
+    <row r="4" spans="1:14" ht="20" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="2"/>
@@ -15616,8 +15632,22 @@
         <v>10</v>
       </c>
       <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="20" customHeight="1">
+    <row r="5" spans="1:14" ht="20" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="27" t="s">
         <v>11</v>
@@ -15638,8 +15668,26 @@
         <v>29.158999999999999</v>
       </c>
       <c r="H5" s="4"/>
+      <c r="I5" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="10">
+        <v>22.917000000000002</v>
+      </c>
+      <c r="L5" s="10">
+        <v>47.723999999999997</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0.26300000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="20" customHeight="1">
+    <row r="6" spans="1:14" ht="20" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="27"/>
       <c r="C6" s="3" t="s">
@@ -15658,8 +15706,24 @@
         <v>24.584</v>
       </c>
       <c r="H6" s="4"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="10">
+        <v>33.18</v>
+      </c>
+      <c r="L6" s="10">
+        <v>30.167000000000002</v>
+      </c>
+      <c r="M6" s="10">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0.29799999999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="20" customHeight="1">
+    <row r="7" spans="1:14" ht="20" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="27"/>
       <c r="C7" s="3" t="s">
@@ -15678,8 +15742,24 @@
         <v>22.512</v>
       </c>
       <c r="H7" s="4"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="10">
+        <v>7.4489999999999998</v>
+      </c>
+      <c r="L7" s="10">
+        <v>22.437000000000001</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0.124</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0.20799999999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" ht="20" customHeight="1">
+    <row r="8" spans="1:14" ht="20" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="27" t="s">
         <v>15</v>
@@ -15700,8 +15780,26 @@
         <v>12.757999999999999</v>
       </c>
       <c r="H8" s="4"/>
+      <c r="I8" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="10">
+        <v>4.6150000000000002</v>
+      </c>
+      <c r="L8" s="10">
+        <v>7.1859999999999999</v>
+      </c>
+      <c r="M8" s="10">
+        <v>11.989000000000001</v>
+      </c>
+      <c r="N8" s="11">
+        <v>14.946</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" ht="20" customHeight="1">
+    <row r="9" spans="1:14" ht="20" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="27"/>
       <c r="C9" s="3" t="s">
@@ -15720,8 +15818,24 @@
         <v>63.664999999999999</v>
       </c>
       <c r="H9" s="4"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="10">
+        <v>31.667000000000002</v>
+      </c>
+      <c r="L9" s="10">
+        <v>52.058999999999997</v>
+      </c>
+      <c r="M9" s="10">
+        <v>63.662999999999997</v>
+      </c>
+      <c r="N9" s="11">
+        <v>65.665000000000006</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" ht="20" customHeight="1">
+    <row r="10" spans="1:14" ht="20" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="27"/>
       <c r="C10" s="3" t="s">
@@ -15740,8 +15854,24 @@
         <v>70.063999999999993</v>
       </c>
       <c r="H10" s="4"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="10">
+        <v>66.153999999999996</v>
+      </c>
+      <c r="L10" s="10">
+        <v>80.388999999999996</v>
+      </c>
+      <c r="M10" s="10">
+        <v>64.933000000000007</v>
+      </c>
+      <c r="N10" s="11">
+        <v>77.671000000000006</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" ht="20" customHeight="1">
+    <row r="11" spans="1:14" ht="20" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="28" t="s">
         <v>17</v>
@@ -15762,8 +15892,26 @@
         <v>56.588999999999999</v>
       </c>
       <c r="H11" s="4"/>
+      <c r="I11" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="10">
+        <v>56.948</v>
+      </c>
+      <c r="L11" s="10">
+        <v>60.081000000000003</v>
+      </c>
+      <c r="M11" s="10">
+        <v>57.103999999999999</v>
+      </c>
+      <c r="N11" s="11">
+        <v>60.347000000000001</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" ht="20" customHeight="1">
+    <row r="12" spans="1:14" ht="20" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="28"/>
       <c r="C12" s="7" t="s">
@@ -15782,8 +15930,24 @@
         <v>63.576000000000001</v>
       </c>
       <c r="H12" s="4"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="10">
+        <v>65.778000000000006</v>
+      </c>
+      <c r="L12" s="10">
+        <v>68.838999999999999</v>
+      </c>
+      <c r="M12" s="10">
+        <v>63.170999999999999</v>
+      </c>
+      <c r="N12" s="11">
+        <v>66.965999999999994</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" ht="20" customHeight="1">
+    <row r="13" spans="1:14" ht="20" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="28"/>
       <c r="C13" s="7" t="s">
@@ -15802,8 +15966,29 @@
         <v>70.769000000000005</v>
       </c>
       <c r="H13" s="4"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="10">
+        <v>78.692999999999998</v>
+      </c>
+      <c r="L13" s="10">
+        <v>74.180000000000007</v>
+      </c>
+      <c r="M13" s="10">
+        <v>66.444000000000003</v>
+      </c>
+      <c r="N13" s="11">
+        <v>74.713999999999999</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" ht="20" customHeight="1">
+    <row r="15" spans="1:14">
+      <c r="B15" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="20" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="2"/>
       <c r="D16" s="25" t="s">
@@ -15839,10 +16024,10 @@
         <v>26</v>
       </c>
       <c r="D18" s="17">
-        <v>672</v>
+        <v>624</v>
       </c>
       <c r="E18" s="17">
-        <v>1226</v>
+        <v>1274</v>
       </c>
       <c r="F18" s="17">
         <v>1497</v>
@@ -15877,10 +16062,10 @@
         <v>26</v>
       </c>
       <c r="D20" s="17">
-        <v>360</v>
+        <v>325</v>
       </c>
       <c r="E20" s="17">
-        <v>633</v>
+        <v>668</v>
       </c>
       <c r="F20" s="17">
         <v>1126</v>
@@ -15945,8 +16130,165 @@
         <v>49.88</v>
       </c>
     </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="5"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="26"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="5"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="17">
+        <v>497</v>
+      </c>
+      <c r="E28" s="17">
+        <v>996</v>
+      </c>
+      <c r="F28" s="17">
+        <v>586</v>
+      </c>
+      <c r="G28" s="18">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="27"/>
+      <c r="C29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="10">
+        <v>57.75</v>
+      </c>
+      <c r="E29" s="10">
+        <v>50.9</v>
+      </c>
+      <c r="F29" s="10">
+        <v>52.56</v>
+      </c>
+      <c r="G29" s="11">
+        <v>50.77</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="17">
+        <v>260</v>
+      </c>
+      <c r="E30" s="17">
+        <v>454</v>
+      </c>
+      <c r="F30" s="17">
+        <v>491</v>
+      </c>
+      <c r="G30" s="18">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="27"/>
+      <c r="C31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="10">
+        <v>65</v>
+      </c>
+      <c r="E31" s="10">
+        <v>48.9</v>
+      </c>
+      <c r="F31" s="10">
+        <v>56.62</v>
+      </c>
+      <c r="G31" s="11">
+        <v>52.85</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="17">
+        <v>604</v>
+      </c>
+      <c r="E32" s="17">
+        <v>742</v>
+      </c>
+      <c r="F32" s="17">
+        <v>1233</v>
+      </c>
+      <c r="G32" s="18">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="28"/>
+      <c r="C33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="10">
+        <v>52.65</v>
+      </c>
+      <c r="E33" s="10">
+        <v>50.13</v>
+      </c>
+      <c r="F33" s="10">
+        <v>56.12</v>
+      </c>
+      <c r="G33" s="11">
+        <v>49.9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="20">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="B18:B19"/>

</xml_diff>

<commit_message>
student level moved to Appendix A
</commit_message>
<xml_diff>
--- a/Code/Graphs.xlsx
+++ b/Code/Graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="540" windowWidth="17480" windowHeight="16420" activeTab="6"/>
+    <workbookView xWindow="13280" yWindow="500" windowWidth="17480" windowHeight="16420" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ASER Results" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="truncated sample" sheetId="4" r:id="rId5"/>
     <sheet name="Truncated Child" sheetId="9" r:id="rId6"/>
     <sheet name="Balance Test" sheetId="2" r:id="rId7"/>
-    <sheet name="viz" sheetId="5" r:id="rId8"/>
-    <sheet name="top 20%" sheetId="6" r:id="rId9"/>
+    <sheet name="appendix" sheetId="10" r:id="rId8"/>
+    <sheet name="viz" sheetId="5" r:id="rId9"/>
+    <sheet name="top 20%" sheetId="6" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'top 20%'!$A$3:$A$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'top 20%'!$A$3:$A$3</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="87">
   <si>
     <t>English</t>
   </si>
@@ -225,6 +226,78 @@
   <si>
     <t>in the consistent schools</t>
   </si>
+  <si>
+    <t>Consistent Treatment Schools</t>
+  </si>
+  <si>
+    <t>Al Rasheed Public School Taleemabad</t>
+  </si>
+  <si>
+    <t>Ferobels House</t>
+  </si>
+  <si>
+    <t>SRM School</t>
+  </si>
+  <si>
+    <t>Al noor School Bhera</t>
+  </si>
+  <si>
+    <t>DOA 12</t>
+  </si>
+  <si>
+    <t>Eloquence Global School</t>
+  </si>
+  <si>
+    <t>Muslim Hands School of Excellence Peshawar</t>
+  </si>
+  <si>
+    <t>Warsak Model School</t>
+  </si>
+  <si>
+    <t>Consistent Control Schools</t>
+  </si>
+  <si>
+    <t>ASER Instrument</t>
+  </si>
+  <si>
+    <t>Learnalicious</t>
+  </si>
+  <si>
+    <t>Peshawar Model School</t>
+  </si>
+  <si>
+    <t>The Real School</t>
+  </si>
+  <si>
+    <t>Rise Model School Daragi Malakand</t>
+  </si>
+  <si>
+    <t>The learner</t>
+  </si>
+  <si>
+    <t>Versatile Education School</t>
+  </si>
+  <si>
+    <t>Al Asr Public School Jutal</t>
+  </si>
+  <si>
+    <t>DOA 19</t>
+  </si>
+  <si>
+    <t>DOA 6</t>
+  </si>
+  <si>
+    <t>Iqra Public School</t>
+  </si>
+  <si>
+    <t>Pak Divisional Public Highschool</t>
+  </si>
+  <si>
+    <t>Quaid-e-azam Public School</t>
+  </si>
+  <si>
+    <t>The Learner</t>
+  </si>
 </sst>
 </file>
 
@@ -349,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -394,6 +467,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,8 +490,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14547,32 +14625,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25">
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="O1" s="24" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="O1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
     </row>
     <row r="2" spans="2:25">
       <c r="B2" s="1"/>
@@ -14843,6 +14921,506 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="20"/>
+      <c r="B1" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="20"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:15" ht="21">
+      <c r="A3" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="20">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="20">
+        <v>3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="20">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" t="s">
+        <v>54</v>
+      </c>
+      <c r="O11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20">
+        <v>2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="20">
+        <v>2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" t="s">
+        <v>55</v>
+      </c>
+      <c r="O17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" t="s">
+        <v>44</v>
+      </c>
+      <c r="O18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="M19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="M20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" t="s">
+        <v>42</v>
+      </c>
+      <c r="O20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="M21" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M6"/>
@@ -14854,24 +15432,24 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="2" spans="2:13">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="24"/>
+      <c r="M2" s="26"/>
     </row>
     <row r="3" spans="2:13">
       <c r="B3" s="1"/>
@@ -15031,14 +15609,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="1"/>
@@ -15133,14 +15711,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="1"/>
@@ -15562,8 +16140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G13"/>
+    <sheetView topLeftCell="A20" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16"/>
@@ -15580,14 +16158,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="D1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="D1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="24" t="s">
         <v>61</v>
       </c>
     </row>
@@ -15595,25 +16173,25 @@
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="4"/>
       <c r="I3" s="5"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25" t="s">
+      <c r="L3" s="27"/>
+      <c r="M3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="26"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:14" ht="20" customHeight="1">
       <c r="A4" s="4"/>
@@ -15649,7 +16227,7 @@
     </row>
     <row r="5" spans="1:14" ht="20" customHeight="1">
       <c r="A5" s="4"/>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -15668,7 +16246,7 @@
         <v>29.158999999999999</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="29" t="s">
         <v>11</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -15689,7 +16267,7 @@
     </row>
     <row r="6" spans="1:14" ht="20" customHeight="1">
       <c r="A6" s="4"/>
-      <c r="B6" s="27"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -15706,7 +16284,7 @@
         <v>24.584</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="27"/>
+      <c r="I6" s="29"/>
       <c r="J6" s="3" t="s">
         <v>13</v>
       </c>
@@ -15725,7 +16303,7 @@
     </row>
     <row r="7" spans="1:14" ht="20" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="27"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
@@ -15742,7 +16320,7 @@
         <v>22.512</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="27"/>
+      <c r="I7" s="29"/>
       <c r="J7" s="3" t="s">
         <v>14</v>
       </c>
@@ -15761,7 +16339,7 @@
     </row>
     <row r="8" spans="1:14" ht="20" customHeight="1">
       <c r="A8" s="4"/>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -15780,7 +16358,7 @@
         <v>12.757999999999999</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="29" t="s">
         <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
@@ -15801,7 +16379,7 @@
     </row>
     <row r="9" spans="1:14" ht="20" customHeight="1">
       <c r="A9" s="4"/>
-      <c r="B9" s="27"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
@@ -15818,7 +16396,7 @@
         <v>63.664999999999999</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="27"/>
+      <c r="I9" s="29"/>
       <c r="J9" s="3" t="s">
         <v>13</v>
       </c>
@@ -15837,7 +16415,7 @@
     </row>
     <row r="10" spans="1:14" ht="20" customHeight="1">
       <c r="A10" s="4"/>
-      <c r="B10" s="27"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
@@ -15854,7 +16432,7 @@
         <v>70.063999999999993</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="27"/>
+      <c r="I10" s="29"/>
       <c r="J10" s="3" t="s">
         <v>14</v>
       </c>
@@ -15873,7 +16451,7 @@
     </row>
     <row r="11" spans="1:14" ht="20" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -15892,7 +16470,7 @@
         <v>56.588999999999999</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="30" t="s">
         <v>17</v>
       </c>
       <c r="J11" s="7" t="s">
@@ -15913,7 +16491,7 @@
     </row>
     <row r="12" spans="1:14" ht="20" customHeight="1">
       <c r="A12" s="4"/>
-      <c r="B12" s="28"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
@@ -15930,7 +16508,7 @@
         <v>63.576000000000001</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="28"/>
+      <c r="I12" s="30"/>
       <c r="J12" s="7" t="s">
         <v>19</v>
       </c>
@@ -15949,7 +16527,7 @@
     </row>
     <row r="13" spans="1:14" ht="20" customHeight="1">
       <c r="A13" s="4"/>
-      <c r="B13" s="28"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="7" t="s">
         <v>20</v>
       </c>
@@ -15966,7 +16544,7 @@
         <v>70.769000000000005</v>
       </c>
       <c r="H13" s="4"/>
-      <c r="I13" s="28"/>
+      <c r="I13" s="30"/>
       <c r="J13" s="7" t="s">
         <v>20</v>
       </c>
@@ -15984,21 +16562,21 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="24" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="20" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="26"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="2:7" ht="20" customHeight="1">
       <c r="B17" s="5"/>
@@ -16017,7 +16595,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="20" customHeight="1">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -16037,7 +16615,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="20" customHeight="1">
-      <c r="B19" s="27"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -16055,7 +16633,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="20" customHeight="1">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -16075,7 +16653,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="20" customHeight="1">
-      <c r="B21" s="27"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="3" t="s">
         <v>27</v>
       </c>
@@ -16093,7 +16671,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="20" customHeight="1">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -16113,7 +16691,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="20" customHeight="1">
-      <c r="B23" s="28"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="3" t="s">
         <v>27</v>
       </c>
@@ -16131,21 +16709,21 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="24" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="5"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25" t="s">
+      <c r="E26" s="27"/>
+      <c r="F26" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="26"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="2:7">
       <c r="B27" s="5"/>
@@ -16164,7 +16742,7 @@
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -16184,7 +16762,7 @@
       </c>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="27"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="3" t="s">
         <v>27</v>
       </c>
@@ -16202,7 +16780,7 @@
       </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -16222,7 +16800,7 @@
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="27"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="3" t="s">
         <v>27</v>
       </c>
@@ -16240,7 +16818,7 @@
       </c>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -16260,7 +16838,7 @@
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="28"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
@@ -16279,26 +16857,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B32:B33"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -16306,6 +16884,191 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:10">
+      <c r="C4" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="G4" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
+      <c r="C8" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
+      <c r="C9" s="34"/>
+      <c r="D9" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10">
+      <c r="C10" s="34"/>
+      <c r="D10" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10">
+      <c r="G11" s="34"/>
+      <c r="H11" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="34"/>
+    </row>
+    <row r="12" spans="3:10">
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J13"/>
   <sheetViews>
@@ -16320,38 +17083,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="25" t="s">
+      <c r="F3" s="28"/>
+      <c r="G3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25" t="s">
+      <c r="H3" s="27"/>
+      <c r="I3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="26"/>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="5"/>
@@ -16382,7 +17145,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -16410,7 +17173,7 @@
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="27"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -16436,7 +17199,7 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="27"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -16462,7 +17225,7 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -16490,7 +17253,7 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="27"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
@@ -16516,7 +17279,7 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="27"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
@@ -16542,7 +17305,7 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -16566,7 +17329,7 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="28"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
@@ -16588,7 +17351,7 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="28"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
@@ -16623,504 +17386,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="20"/>
-      <c r="B1" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="20"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="20"/>
-    </row>
-    <row r="3" spans="1:15" ht="21">
-      <c r="A3" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20">
-        <v>5</v>
-      </c>
-      <c r="M5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="20">
-        <v>4</v>
-      </c>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="20">
-        <v>3</v>
-      </c>
-      <c r="M7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="20">
-        <v>3</v>
-      </c>
-      <c r="M8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20">
-        <v>3</v>
-      </c>
-      <c r="M9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" t="s">
-        <v>43</v>
-      </c>
-      <c r="O9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20">
-        <v>2</v>
-      </c>
-      <c r="M11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11" t="s">
-        <v>54</v>
-      </c>
-      <c r="O11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20">
-        <v>2</v>
-      </c>
-      <c r="M12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" t="s">
-        <v>38</v>
-      </c>
-      <c r="O12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="20">
-        <v>2</v>
-      </c>
-      <c r="M13" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>38</v>
-      </c>
-      <c r="N14" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>35</v>
-      </c>
-      <c r="N15" t="s">
-        <v>42</v>
-      </c>
-      <c r="O15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>52</v>
-      </c>
-      <c r="N17" t="s">
-        <v>55</v>
-      </c>
-      <c r="O17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>32</v>
-      </c>
-      <c r="N18" t="s">
-        <v>44</v>
-      </c>
-      <c r="O18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="M19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N19" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="M20" t="s">
-        <v>34</v>
-      </c>
-      <c r="N20" t="s">
-        <v>42</v>
-      </c>
-      <c r="O20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="M21" t="s">
-        <v>39</v>
-      </c>
-      <c r="N21" t="s">
-        <v>33</v>
-      </c>
-      <c r="O21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
limittaion, conclusion and appendix B
</commit_message>
<xml_diff>
--- a/Code/Graphs.xlsx
+++ b/Code/Graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13280" yWindow="500" windowWidth="17480" windowHeight="16420" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="3180" yWindow="500" windowWidth="17480" windowHeight="16420" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ASER Results" sheetId="1" r:id="rId1"/>
@@ -16887,8 +16887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>